<commit_message>
Formatting Changes - "Second Commit"
</commit_message>
<xml_diff>
--- a/Week of July 9 2023/Day 2/Personal Expensive Tracker.xlsx
+++ b/Week of July 9 2023/Day 2/Personal Expensive Tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbriody/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbriody/Desktop/Coding Temple/Data-Analytics-Projects/Week of July 9 2023/Day 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61452B99-8035-DC4B-B3A3-85CBEBE025C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF6487B-05D3-BC4F-806D-86FB70CEFE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="500" windowWidth="49120" windowHeight="25480" xr2:uid="{2A1F9988-2C7F-0840-8694-CFE454CA8625}"/>
   </bookViews>
@@ -22,10 +22,10 @@
   <definedNames>
     <definedName name="NativeTimeline_Date">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="166" r:id="rId6"/>
-    <pivotCache cacheId="181" r:id="rId7"/>
+    <pivotCache cacheId="184" r:id="rId6"/>
+    <pivotCache cacheId="185" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -191,8 +191,8 @@
   <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="[$-409]mmm\-yy;@"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -238,15 +238,57 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -254,18 +296,132 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,27 +430,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5407,8 +5619,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" Requires="tsle">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
+      <mc:Choice Requires="tsle">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="22" name="Date">
@@ -5426,12 +5638,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
-              <tsle:timeslicer xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" name="Date"/>
+              <tsle:timeslicer name="Date"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -5687,7 +5899,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alexander H. Briody" refreshedDate="45118.847945254631" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="1" xr:uid="{A4BE0FBC-0D1F-2A4C-8BB2-DA7C089F382A}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A13:C14" sheet="Expense Tracker"/>
+    <worksheetSource ref="A14:C15" sheet="Expense Tracker"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Max" numFmtId="6">
@@ -5717,7 +5929,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alexander H. Briody" refreshedDate="45118.853458796293" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="7" xr:uid="{E035C8E1-51A6-CD40-B8BE-B40710CF8AD0}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:O9" sheet="Expense Tracker"/>
+    <worksheetSource ref="A3:O10" sheet="Expense Tracker"/>
   </cacheSource>
   <cacheFields count="16">
     <cacheField name="Date" numFmtId="0">
@@ -6107,7 +6319,7 @@
     <cacheField name="Budget Allocation" numFmtId="6">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4000" maxValue="4000"/>
     </cacheField>
-    <cacheField name="Surplus from Previous Month" numFmtId="177">
+    <cacheField name="Surplus from Previous Month" numFmtId="165">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="107"/>
     </cacheField>
     <cacheField name="Housing" numFmtId="6">
@@ -6377,7 +6589,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFBABC3D-A316-F743-A81A-20040C04F92B}" name="PivotTable38" cacheId="166" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFBABC3D-A316-F743-A81A-20040C04F92B}" name="PivotTable38" cacheId="184" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:C4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="3">
     <pivotField dataField="1" numFmtId="6" showAll="0">
@@ -6417,7 +6629,7 @@
     </i>
   </colItems>
   <dataFields count="3">
-    <dataField name="Avg Monthly Expenses" fld="2" baseField="0" baseItem="0" numFmtId="177"/>
+    <dataField name="Avg Monthly Expenses" fld="2" baseField="0" baseItem="0" numFmtId="165"/>
     <dataField name="Max Monthly Expenses" fld="0" baseField="0" baseItem="0"/>
     <dataField name="Min Monthly Expenses" fld="1" subtotal="min" baseField="0" baseItem="0"/>
   </dataFields>
@@ -6463,7 +6675,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA2E3341-B082-1B4D-B78B-838CE514C666}" name="PivotTable39" cacheId="181" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA2E3341-B082-1B4D-B78B-838CE514C666}" name="PivotTable39" cacheId="185" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:I11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0">
@@ -6840,7 +7052,7 @@
       </items>
     </pivotField>
     <pivotField numFmtId="6" showAll="0"/>
-    <pivotField numFmtId="177" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
     <pivotField numFmtId="6" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -7117,7 +7329,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{82A90FC2-F45C-CA45-861D-47AF1C1F70CE}" name="PivotTable40" cacheId="181" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{82A90FC2-F45C-CA45-861D-47AF1C1F70CE}" name="PivotTable40" cacheId="185" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0">
@@ -7494,7 +7706,7 @@
       </items>
     </pivotField>
     <pivotField numFmtId="6" showAll="0"/>
-    <pivotField numFmtId="177" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
     <pivotField numFmtId="6" showAll="0"/>
     <pivotField numFmtId="6" showAll="0"/>
     <pivotField numFmtId="6" showAll="0"/>
@@ -7944,7 +8156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E07F71-9630-2740-ABAE-AACAEE9F5228}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
@@ -7964,10 +8176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D9E9E2-CF8E-0646-B297-0D3AB9E6B095}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7987,488 +8199,499 @@
     <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:15" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:15" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O3" s="32" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
-        <v>44927</v>
-      </c>
-      <c r="B3" s="6">
-        <v>4000</v>
-      </c>
-      <c r="C3" s="14">
-        <v>42</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E3" s="1">
-        <v>278</v>
-      </c>
-      <c r="F3" s="1">
-        <v>288</v>
-      </c>
-      <c r="G3" s="1">
-        <v>433</v>
-      </c>
-      <c r="H3" s="1">
-        <v>323</v>
-      </c>
-      <c r="I3" s="1">
-        <v>258</v>
-      </c>
-      <c r="J3" s="1">
-        <v>87</v>
-      </c>
-      <c r="K3" s="1">
-        <v>65</v>
-      </c>
-      <c r="L3" s="1">
-        <v>400</v>
-      </c>
-      <c r="M3" s="1">
-        <v>354</v>
-      </c>
-      <c r="N3" s="13">
-        <f>SUM(D3:M3)</f>
-        <v>3986</v>
-      </c>
-      <c r="O3" s="13">
-        <f>(B3+C3)-N3</f>
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
-        <v>44958</v>
-      </c>
-      <c r="B4" s="6">
+        <v>44927</v>
+      </c>
+      <c r="B4" s="13">
         <v>4000</v>
       </c>
-      <c r="C4" s="15">
-        <f>IF(O3&gt;0, O3,0)</f>
+      <c r="C4" s="14">
+        <v>42</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1500</v>
+      </c>
+      <c r="E4" s="16">
+        <v>278</v>
+      </c>
+      <c r="F4" s="15">
+        <v>288</v>
+      </c>
+      <c r="G4" s="16">
+        <v>433</v>
+      </c>
+      <c r="H4" s="15">
+        <v>323</v>
+      </c>
+      <c r="I4" s="16">
+        <v>258</v>
+      </c>
+      <c r="J4" s="15">
+        <v>87</v>
+      </c>
+      <c r="K4" s="16">
+        <v>65</v>
+      </c>
+      <c r="L4" s="15">
+        <v>400</v>
+      </c>
+      <c r="M4" s="16">
+        <v>354</v>
+      </c>
+      <c r="N4" s="17">
+        <f>SUM(D4:M4)</f>
+        <v>3986</v>
+      </c>
+      <c r="O4" s="33">
+        <f>(B4+C4)-N4</f>
         <v>56</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>284</v>
-      </c>
-      <c r="F4" s="1">
-        <v>273</v>
-      </c>
-      <c r="G4" s="1">
-        <v>329</v>
-      </c>
-      <c r="H4" s="1">
-        <v>257</v>
-      </c>
-      <c r="I4" s="1">
-        <v>258</v>
-      </c>
-      <c r="J4" s="1">
-        <v>87</v>
-      </c>
-      <c r="K4" s="1">
-        <v>36</v>
-      </c>
-      <c r="L4" s="1">
-        <v>400</v>
-      </c>
-      <c r="M4" s="1">
-        <v>525</v>
-      </c>
-      <c r="N4" s="13">
-        <f t="shared" ref="N4:N9" si="0">SUM(D4:M4)</f>
-        <v>3949</v>
-      </c>
-      <c r="O4" s="13">
-        <f t="shared" ref="O4:O9" si="1">(B4+C4)-N4</f>
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
-        <v>44986</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="18">
+        <v>44958</v>
+      </c>
+      <c r="B5" s="13">
         <v>4000</v>
       </c>
-      <c r="C5" s="15">
-        <f>IF(O4&gt;0, O4,0)</f>
+      <c r="C5" s="19">
+        <f t="shared" ref="C5:C10" si="0">IF(O4&gt;0, O4,0)</f>
+        <v>56</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1500</v>
+      </c>
+      <c r="E5" s="16">
+        <v>284</v>
+      </c>
+      <c r="F5" s="15">
+        <v>273</v>
+      </c>
+      <c r="G5" s="16">
+        <v>329</v>
+      </c>
+      <c r="H5" s="15">
+        <v>257</v>
+      </c>
+      <c r="I5" s="16">
+        <v>258</v>
+      </c>
+      <c r="J5" s="15">
+        <v>87</v>
+      </c>
+      <c r="K5" s="16">
+        <v>36</v>
+      </c>
+      <c r="L5" s="15">
+        <v>400</v>
+      </c>
+      <c r="M5" s="16">
+        <v>525</v>
+      </c>
+      <c r="N5" s="17">
+        <f t="shared" ref="N5:N10" si="1">SUM(D5:M5)</f>
+        <v>3949</v>
+      </c>
+      <c r="O5" s="33">
+        <f t="shared" ref="O5:O10" si="2">(B5+C5)-N5</f>
         <v>107</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>267</v>
-      </c>
-      <c r="F5" s="1">
-        <v>292</v>
-      </c>
-      <c r="G5" s="1">
-        <v>365</v>
-      </c>
-      <c r="H5" s="1">
-        <v>452</v>
-      </c>
-      <c r="I5" s="1">
-        <v>258</v>
-      </c>
-      <c r="J5" s="1">
-        <v>154</v>
-      </c>
-      <c r="K5" s="1">
-        <v>23</v>
-      </c>
-      <c r="L5" s="1">
-        <v>400</v>
-      </c>
-      <c r="M5" s="1">
-        <v>636</v>
-      </c>
-      <c r="N5" s="13">
-        <f t="shared" si="0"/>
-        <v>4347</v>
-      </c>
-      <c r="O5" s="13">
-        <f t="shared" si="1"/>
-        <v>-240</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
-        <v>45017</v>
-      </c>
-      <c r="B6" s="6">
+        <v>44986</v>
+      </c>
+      <c r="B6" s="13">
         <v>4000</v>
       </c>
-      <c r="C6" s="15">
-        <f>IF(O5&gt;0, O5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="19">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="D6" s="15">
         <v>1500</v>
       </c>
-      <c r="E6" s="1">
-        <v>256</v>
-      </c>
-      <c r="F6" s="1">
-        <v>367</v>
-      </c>
-      <c r="G6" s="1">
-        <v>465</v>
-      </c>
-      <c r="H6" s="1">
-        <v>176</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="E6" s="16">
+        <v>267</v>
+      </c>
+      <c r="F6" s="15">
+        <v>292</v>
+      </c>
+      <c r="G6" s="16">
+        <v>365</v>
+      </c>
+      <c r="H6" s="15">
+        <v>452</v>
+      </c>
+      <c r="I6" s="16">
         <v>258</v>
       </c>
-      <c r="J6" s="1">
-        <v>87</v>
-      </c>
-      <c r="K6" s="1">
-        <v>58</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="J6" s="15">
+        <v>154</v>
+      </c>
+      <c r="K6" s="16">
+        <v>23</v>
+      </c>
+      <c r="L6" s="15">
         <v>400</v>
       </c>
-      <c r="M6" s="1">
-        <v>345</v>
-      </c>
-      <c r="N6" s="13">
-        <f t="shared" si="0"/>
-        <v>3912</v>
-      </c>
-      <c r="O6" s="13">
+      <c r="M6" s="16">
+        <v>636</v>
+      </c>
+      <c r="N6" s="17">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>4347</v>
+      </c>
+      <c r="O6" s="33">
+        <f t="shared" si="2"/>
+        <v>-240</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
-        <v>45047</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="18">
+        <v>45017</v>
+      </c>
+      <c r="B7" s="13">
         <v>4000</v>
       </c>
-      <c r="C7" s="15">
-        <f>IF(O6&gt;0, O6,0)</f>
+      <c r="C7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1500</v>
+      </c>
+      <c r="E7" s="16">
+        <v>256</v>
+      </c>
+      <c r="F7" s="15">
+        <v>367</v>
+      </c>
+      <c r="G7" s="16">
+        <v>465</v>
+      </c>
+      <c r="H7" s="15">
+        <v>176</v>
+      </c>
+      <c r="I7" s="16">
+        <v>258</v>
+      </c>
+      <c r="J7" s="15">
+        <v>87</v>
+      </c>
+      <c r="K7" s="16">
+        <v>58</v>
+      </c>
+      <c r="L7" s="15">
+        <v>400</v>
+      </c>
+      <c r="M7" s="16">
+        <v>345</v>
+      </c>
+      <c r="N7" s="17">
+        <f t="shared" si="1"/>
+        <v>3912</v>
+      </c>
+      <c r="O7" s="33">
+        <f t="shared" si="2"/>
         <v>88</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1500</v>
-      </c>
-      <c r="E7" s="1">
-        <v>266</v>
-      </c>
-      <c r="F7" s="1">
-        <v>482</v>
-      </c>
-      <c r="G7" s="1">
-        <v>376</v>
-      </c>
-      <c r="H7" s="1">
-        <v>279</v>
-      </c>
-      <c r="I7" s="1">
-        <v>258</v>
-      </c>
-      <c r="J7" s="1">
-        <v>132</v>
-      </c>
-      <c r="K7" s="1">
-        <v>245</v>
-      </c>
-      <c r="L7" s="1">
-        <v>400</v>
-      </c>
-      <c r="M7" s="1">
-        <v>635</v>
-      </c>
-      <c r="N7" s="13">
-        <f t="shared" si="0"/>
-        <v>4573</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="1"/>
-        <v>-485</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
-        <v>45078</v>
-      </c>
-      <c r="B8" s="6">
+        <v>45047</v>
+      </c>
+      <c r="B8" s="13">
         <v>4000</v>
       </c>
-      <c r="C8" s="15">
-        <f>IF(O7&gt;0, O7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="19">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="D8" s="15">
         <v>1500</v>
       </c>
-      <c r="E8" s="1">
-        <v>274</v>
-      </c>
-      <c r="F8" s="1">
-        <v>273</v>
-      </c>
-      <c r="G8" s="1">
-        <v>453</v>
-      </c>
-      <c r="H8" s="1">
-        <v>154</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="E8" s="16">
+        <v>266</v>
+      </c>
+      <c r="F8" s="15">
+        <v>482</v>
+      </c>
+      <c r="G8" s="16">
+        <v>376</v>
+      </c>
+      <c r="H8" s="15">
+        <v>279</v>
+      </c>
+      <c r="I8" s="16">
         <v>258</v>
       </c>
-      <c r="J8" s="1">
-        <v>233</v>
-      </c>
-      <c r="K8" s="1">
-        <v>378</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="J8" s="15">
+        <v>132</v>
+      </c>
+      <c r="K8" s="16">
+        <v>245</v>
+      </c>
+      <c r="L8" s="15">
         <v>400</v>
       </c>
-      <c r="M8" s="1">
-        <v>358</v>
-      </c>
-      <c r="N8" s="13">
-        <f t="shared" si="0"/>
-        <v>4281</v>
-      </c>
-      <c r="O8" s="13">
+      <c r="M8" s="16">
+        <v>635</v>
+      </c>
+      <c r="N8" s="17">
         <f t="shared" si="1"/>
-        <v>-281</v>
+        <v>4573</v>
+      </c>
+      <c r="O8" s="33">
+        <f t="shared" si="2"/>
+        <v>-485</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+      <c r="A9" s="18">
+        <v>45078</v>
+      </c>
+      <c r="B9" s="13">
+        <v>4000</v>
+      </c>
+      <c r="C9" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1500</v>
+      </c>
+      <c r="E9" s="16">
+        <v>274</v>
+      </c>
+      <c r="F9" s="15">
+        <v>273</v>
+      </c>
+      <c r="G9" s="16">
+        <v>453</v>
+      </c>
+      <c r="H9" s="15">
+        <v>154</v>
+      </c>
+      <c r="I9" s="16">
+        <v>258</v>
+      </c>
+      <c r="J9" s="15">
+        <v>233</v>
+      </c>
+      <c r="K9" s="16">
+        <v>378</v>
+      </c>
+      <c r="L9" s="15">
+        <v>400</v>
+      </c>
+      <c r="M9" s="16">
+        <v>358</v>
+      </c>
+      <c r="N9" s="17">
+        <f t="shared" si="1"/>
+        <v>4281</v>
+      </c>
+      <c r="O9" s="33">
+        <f t="shared" si="2"/>
+        <v>-281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
         <v>45108</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B10" s="21">
         <v>4000</v>
       </c>
-      <c r="C9" s="15">
-        <f>IF(O8&gt;0, O8,0)</f>
+      <c r="C10" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="23">
         <v>1500</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="24">
         <v>298</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="23">
         <v>124</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G10" s="24">
         <v>175</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H10" s="23">
         <v>98</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I10" s="24">
         <v>258</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J10" s="23">
         <v>87</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K10" s="24">
         <v>25</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L10" s="23">
         <v>400</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M10" s="24">
         <v>125</v>
       </c>
-      <c r="N9" s="13">
-        <f t="shared" si="0"/>
+      <c r="N10" s="25">
+        <f t="shared" si="1"/>
         <v>3090</v>
       </c>
-      <c r="O9" s="13">
-        <f t="shared" si="1"/>
+      <c r="O10" s="34">
+        <f t="shared" si="2"/>
         <v>910</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="47" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="18">
-        <f>MAX(N3:N9)</f>
+      <c r="A14" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="53">
+        <f>MAX(N4:N10)</f>
         <v>4573</v>
       </c>
-      <c r="B14" s="18">
-        <f>MIN(N3:N9)</f>
+      <c r="B15" s="54">
+        <f>MIN(N4:N10)</f>
         <v>3090</v>
       </c>
-      <c r="C14" s="18">
-        <f>AVERAGE(N3:N9)</f>
+      <c r="C15" s="55">
+        <f>AVERAGE(N4:N10)</f>
         <v>4019.7142857142858</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="20">
-        <f>MAX(O3:O9)</f>
+      <c r="A18" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="44">
+        <f>MAX(O4:O10)</f>
         <v>910</v>
       </c>
-      <c r="B18" s="18">
-        <f>MIN(O3:O9)</f>
+      <c r="B19" s="45">
+        <f>MIN(O4:O10)</f>
         <v>-485</v>
       </c>
-      <c r="C18" s="18">
-        <f>AVERAGE(O3:O9)</f>
+      <c r="C19" s="46">
+        <f>AVERAGE(O4:O10)</f>
         <v>22.142857142857142</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8503,13 +8726,13 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
+      <c r="A4" s="8">
         <v>4019.7142857142858</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>4573</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>3090</v>
       </c>
     </row>
@@ -8539,7 +8762,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
@@ -8568,234 +8791,234 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="9">
         <v>278</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>288</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <v>433</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>323</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="5">
         <v>258</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <v>87</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="5">
         <v>65</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="5">
         <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="9">
         <v>284</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>273</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <v>329</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>257</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="5">
         <v>258</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>87</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="5">
         <v>36</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="5">
         <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="9">
         <v>267</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>292</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="5">
         <v>365</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>452</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="5">
         <v>258</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>154</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="5">
         <v>23</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="5">
         <v>636</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="9">
         <v>256</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>367</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>465</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <v>176</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="5">
         <v>258</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <v>87</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="5">
         <v>58</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="5">
         <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="9">
         <v>266</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <v>482</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="5">
         <v>376</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>279</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="5">
         <v>258</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <v>132</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="5">
         <v>245</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="5">
         <v>635</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="9">
         <v>274</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>273</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="5">
         <v>453</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="5">
         <v>154</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="5">
         <v>258</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <v>233</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="5">
         <v>378</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="5">
         <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="9">
         <v>298</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>124</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="5">
         <v>175</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="5">
         <v>98</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="5">
         <v>258</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <v>87</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="5">
         <v>25</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="5">
         <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="9">
         <v>1923</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="5">
         <v>2099</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="5">
         <v>2596</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="5">
         <v>1739</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="5">
         <v>1806</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="5">
         <v>867</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="5">
         <v>830</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="5">
         <v>2978</v>
       </c>
     </row>
@@ -8819,74 +9042,74 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="9">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="9">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="9">
         <v>-240</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="9">
         <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="9">
         <v>-485</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="9">
         <v>-281</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="9">
         <v>910</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="9">
         <v>155</v>
       </c>
     </row>

</xml_diff>